<commit_message>
Added DeleteExcelFile workflow to delete the excel file after it was sent, integrated it in SaveQueryAndSendByMail, updated SendFileByExvel and WriteTableToExcel
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://futureworkforcecompany-my.sharepoint.com/personal/diana_gradinaru_fwfcompany_com/Documents/Documents/POCs/APIs_and_db/APIs_and_db_Performer/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://futureworkforcecompany-my.sharepoint.com/personal/diana_gradinaru_fwfcompany_com/Documents/Documents/UiPath/APIs_and_db_Performer/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB17C26E-F11E-409C-8EA0-DA0DCBABDCD4}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0CA6EFF-E50E-4955-8C7A-7700ED953D1D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -177,9 +177,6 @@
   </si>
   <si>
     <t>Email address to send the excel file to.</t>
-  </si>
-  <si>
-    <t>strEmailBody</t>
   </si>
   <si>
     <t>Hello,
@@ -191,13 +188,25 @@
     <t>Email body</t>
   </si>
   <si>
-    <t>strEmailSubjct</t>
-  </si>
-  <si>
     <t>The requested movies</t>
   </si>
   <si>
     <t>Email subject</t>
+  </si>
+  <si>
+    <t>strEmailBodyNoFile</t>
+  </si>
+  <si>
+    <t>strEmailSubject</t>
+  </si>
+  <si>
+    <t>Hello,
+The database does not contain any movies with the string '{0}' in their title.
+Regards, 
+Diana</t>
+  </si>
+  <si>
+    <t>strEmailBodyWithFile</t>
   </si>
 </sst>
 </file>
@@ -574,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -681,28 +690,35 @@
     </row>
     <row r="11" spans="1:26" ht="87.6" customHeight="1">
       <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" t="s">
         <v>52</v>
-      </c>
-      <c r="C11" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.4">
       <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
         <v>54</v>
-      </c>
-      <c r="B12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="86.4">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
@@ -1686,7 +1702,6 @@
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Removed InitAllApplications since it's not needed
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://futureworkforcecompany-my.sharepoint.com/personal/diana_gradinaru_fwfcompany_com/Documents/Documents/UiPath/APIs_and_db_Performer/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://futureworkforcecompany-my.sharepoint.com/personal/diana_gradinaru_fwfcompany_com/Documents/Documents/POCs/APIs_and_db/Dispatcher and Performer/APIs_and_db_Performer/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0CA6EFF-E50E-4955-8C7A-7700ED953D1D}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C55F9A77-B61B-4B42-BAFA-76D3EFB4795D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -173,9 +173,6 @@
     <t>strEmailAddressSendTo</t>
   </si>
   <si>
-    <t>diana.gradinaru@fwfcompany.com</t>
-  </si>
-  <si>
     <t>Email address to send the excel file to.</t>
   </si>
   <si>
@@ -207,13 +204,16 @@
   </si>
   <si>
     <t>strEmailBodyWithFile</t>
+  </si>
+  <si>
+    <t>diana.gradinaru@fwfcompany.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -238,6 +238,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -256,21 +262,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -585,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -681,42 +690,42 @@
       <c r="A10" t="s">
         <v>48</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
         <v>49</v>
-      </c>
-      <c r="C10" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="87.6" customHeight="1">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
         <v>51</v>
-      </c>
-      <c r="C11" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.4">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
         <v>53</v>
-      </c>
-      <c r="C12" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="86.4">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1704,8 +1713,11 @@
     <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{E9622000-77CF-4AD3-9A0C-6D402F9822B6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>